<commit_message>
added functionality of changing contact person
</commit_message>
<xml_diff>
--- a/ProductExcelApp/Excel documents/Products.xlsx
+++ b/ProductExcelApp/Excel documents/Products.xlsx
@@ -146,7 +146,7 @@
     <x:t>Муравьёвa Жанна Львовна</x:t>
   </x:si>
   <x:si>
-    <x:t>Андреев Кирилл Дмитриевич</x:t>
+    <x:t>Андреев Андрей Дмитриевич</x:t>
   </x:si>
   <x:si>
     <x:t>Литр</x:t>
@@ -807,185 +807,185 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>287</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>820</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>748</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>633</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:dimension ref="A1:D20"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A5" sqref="A5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <x:col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <x:col min="3" max="3" width="55.28515625" customWidth="1"/>
+    <x:col min="4" max="4" width="40.7109375" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="1">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D2" s="1" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="1">
+        <x:v>820</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D3" s="1" t="s">
+        <x:v>39</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="1">
+        <x:v>748</x:v>
+      </x:c>
+      <x:c r="B4" s="1" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C4" s="1" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D4" s="1" t="s">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="1">
+        <x:v>633</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C5" s="1" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D5" s="1" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="1"/>
+      <x:c r="B6" s="1"/>
+      <x:c r="C6" s="1"/>
+      <x:c r="D6" s="1"/>
+    </x:row>
+    <x:row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="1"/>
+      <x:c r="B7" s="1"/>
+      <x:c r="C7" s="1"/>
+      <x:c r="D7" s="1"/>
+    </x:row>
+    <x:row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="1"/>
+      <x:c r="B8" s="1"/>
+      <x:c r="C8" s="1"/>
+      <x:c r="D8" s="1"/>
+    </x:row>
+    <x:row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="1"/>
+      <x:c r="B9" s="1"/>
+      <x:c r="C9" s="1"/>
+      <x:c r="D9" s="1"/>
+    </x:row>
+    <x:row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="1"/>
+      <x:c r="B10" s="1"/>
+      <x:c r="C10" s="1"/>
+      <x:c r="D10" s="1"/>
+    </x:row>
+    <x:row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="1"/>
+      <x:c r="B11" s="1"/>
+      <x:c r="C11" s="1"/>
+      <x:c r="D11" s="1"/>
+    </x:row>
+    <x:row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="1"/>
+      <x:c r="B12" s="1"/>
+      <x:c r="C12" s="1"/>
+      <x:c r="D12" s="1"/>
+    </x:row>
+    <x:row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="1"/>
+      <x:c r="B13" s="1"/>
+      <x:c r="C13" s="1"/>
+      <x:c r="D13" s="1"/>
+    </x:row>
+    <x:row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="1"/>
+      <x:c r="B14" s="1"/>
+      <x:c r="C14" s="1"/>
+      <x:c r="D14" s="1"/>
+    </x:row>
+    <x:row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A15" s="1"/>
+      <x:c r="B15" s="1"/>
+      <x:c r="C15" s="1"/>
+      <x:c r="D15" s="1"/>
+    </x:row>
+    <x:row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A16" s="1"/>
+      <x:c r="B16" s="1"/>
+      <x:c r="C16" s="1"/>
+      <x:c r="D16" s="1"/>
+    </x:row>
+    <x:row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A17" s="1"/>
+      <x:c r="B17" s="1"/>
+      <x:c r="C17" s="1"/>
+      <x:c r="D17" s="1"/>
+    </x:row>
+    <x:row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A18" s="1"/>
+      <x:c r="B18" s="1"/>
+      <x:c r="C18" s="1"/>
+      <x:c r="D18" s="1"/>
+    </x:row>
+    <x:row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A19" s="1"/>
+      <x:c r="B19" s="1"/>
+      <x:c r="C19" s="1"/>
+      <x:c r="D19" s="1"/>
+    </x:row>
+    <x:row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <x:c r="A20" s="1"/>
+      <x:c r="B20" s="1"/>
+      <x:c r="C20" s="1"/>
+      <x:c r="D20" s="1"/>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>